<commit_message>
New feature and sprints
</commit_message>
<xml_diff>
--- a/task.xlsx
+++ b/task.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Raul\PycharmProjects\pythonProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E39C4821-BB53-4C2E-8C60-2F85BD4B5B84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5E8B6B2-C08A-4874-B5EB-D8BD0BB7C5F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{4B2B56B1-63B4-4DD6-8DB2-4E37F33374C4}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
   <si>
     <t>iOS</t>
   </si>
@@ -101,6 +101,12 @@
   </si>
   <si>
     <t>[Acessib] And Activiter IDL</t>
+  </si>
+  <si>
+    <t>Bugs</t>
+  </si>
+  <si>
+    <t>20/06/2023 - 25/06/2023</t>
   </si>
 </sst>
 </file>
@@ -456,10 +462,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2FAF675-CE6C-48FD-9AB4-BD7BAD23FBFB}">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6:E7"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -475,7 +481,7 @@
     <col min="9" max="9" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -503,8 +509,11 @@
       <c r="I1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="J1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -529,8 +538,11 @@
       <c r="H2" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -556,7 +568,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -582,7 +594,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -603,7 +615,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -627,7 +639,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -651,22 +663,22 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>

</xml_diff>